<commit_message>
removing the evaluation of the models in the original questons df
</commit_message>
<xml_diff>
--- a/input/Questions.xlsx
+++ b/input/Questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vanes\OneDrive\Área de Trabalho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\docs\Fgv\7p_projetos\Search_Engine\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9641EC6D-340C-4358-803D-A1400BB2C368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97153663-2FE0-4929-AB34-C2261B762C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -414,17 +414,17 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A13" sqref="A13:C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="30.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" customWidth="1"/>
-    <col min="3" max="3" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.88671875" customWidth="1"/>
+    <col min="3" max="3" width="37.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -435,7 +435,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -446,7 +446,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -457,7 +457,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -468,7 +468,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -479,7 +479,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -490,7 +490,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -501,7 +501,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -512,7 +512,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -523,7 +523,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -534,7 +534,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -545,7 +545,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -556,7 +556,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D16" s="1"/>
     </row>
   </sheetData>

</xml_diff>